<commit_message>
E:\project_3\16-07-2024\project\search_body_no.py whole code is commented ,this code were imported in home_screen,delete_screen but,now search_by_body_no(body_no, main_frame) this function is added into home_screen,delete_screen,backup_screen
</commit_message>
<xml_diff>
--- a/import/import_box.xlsx
+++ b/import/import_box.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project_3\16-07-2024\project\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D7DFE5-DFF4-4A72-B038-2A9DBA7DE0C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1F49AA-8169-44F1-8C7E-E901CFC1482E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{D8515151-6164-46AA-87F0-3D4D4A61D199}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="13">
   <si>
     <t>BODY</t>
   </si>
@@ -70,6 +70,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -145,6 +148,12 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -460,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB59ED08-7205-4B0F-8A26-8A56E0B90DBA}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,7 +490,7 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D1" s="3"/>
@@ -501,7 +510,7 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="8">
         <v>1</v>
       </c>
       <c r="D2" s="6"/>
@@ -510,13 +519,13 @@
     </row>
     <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
-        <v>2406169</v>
+        <v>24061691</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4">
-        <v>11</v>
+      <c r="C3" s="8">
+        <v>2</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6"/>
@@ -529,8 +538,8 @@
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4">
-        <v>6</v>
+      <c r="C4" s="8">
+        <v>3</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -543,8 +552,8 @@
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4">
-        <v>3</v>
+      <c r="C5" s="8">
+        <v>4</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -552,13 +561,13 @@
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
-        <v>2406161</v>
+        <v>24061612</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4">
-        <v>2</v>
+      <c r="C6" s="8">
+        <v>5</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -571,8 +580,8 @@
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4">
-        <v>4</v>
+      <c r="C7" s="8">
+        <v>6</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -585,8 +594,8 @@
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="4">
-        <v>15</v>
+      <c r="C8" s="8">
+        <v>7</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -599,8 +608,8 @@
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="4">
-        <v>20</v>
+      <c r="C9" s="8">
+        <v>8</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -613,8 +622,8 @@
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4">
-        <v>14</v>
+      <c r="C10" s="8">
+        <v>9</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -622,17 +631,451 @@
     </row>
     <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
-        <v>2406144</v>
+        <v>2406145</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="4">
-        <v>19</v>
+      <c r="C11" s="8">
+        <v>10</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2406146</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>24061463</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>2406147</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2406148</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>2406149</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2406150</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>2406151</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>2406152</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>2406153</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>2406154</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>2406155</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>2406156</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>2406157</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>2406158</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>2406159</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>2406160</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>2406161</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>2406162</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>2406163</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>2406164</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>2406165</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>2406166</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>2406167</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>2406168</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>2406169</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>2406170</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>2406171</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>2406172</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>2406173</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>2406174</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>2406175</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>2406176</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>2406177</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>2406178</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>2406179</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>2406180</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>2406181</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>2406182</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>2406183</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C51">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
final code working 05-09-2024
</commit_message>
<xml_diff>
--- a/import/import_box.xlsx
+++ b/import/import_box.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project_3\16-07-2024\project\import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\05-09-2024\Avani-Industry-Kolhapur\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F61C16-C738-4F31-9A5F-6EE261658C73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E070288E-0A71-4AC5-9DB5-BF3175DBBA8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{D8515151-6164-46AA-87F0-3D4D4A61D199}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>BODY</t>
   </si>
@@ -99,7 +99,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -122,11 +122,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -144,6 +155,9 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -460,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB59ED08-7205-4B0F-8A26-8A56E0B90DBA}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,6 +607,28 @@
         <v>9</v>
       </c>
     </row>
+    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
+        <v>2406038</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5">
+        <v>2406039</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="7">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>